<commit_message>
Add digital folder number field to SA templates
</commit_message>
<xml_diff>
--- a/ExceltoMODSWF/SA-MODS-template.xlsx
+++ b/ExceltoMODSWF/SA-MODS-template.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26327"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26501"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://adminliveunc-my.sharepoint.com/personal/goslen_ad_unc_edu/Documents/Desktop/update-sa-templates/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\goslen\git_repos\box-c-mods-templates\ExceltoMODSWF\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="175" documentId="13_ncr:1_{96006D6A-0EE2-40AB-9B61-D08C696F0DB6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{AADAE6D2-0FCD-45B1-AEBB-1F966E4BB486}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{74121E21-8FC5-4C4D-9440-02A756289549}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{30AE1F1C-9D6D-4975-B041-019DDB28DD50}"/>
+    <workbookView xWindow="1845" yWindow="705" windowWidth="24180" windowHeight="14115" activeTab="1" xr2:uid="{30AE1F1C-9D6D-4975-B041-019DDB28DD50}"/>
   </bookViews>
   <sheets>
     <sheet name="Template" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="141" uniqueCount="92">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="95">
   <si>
     <t>Contributor (Participant) Name</t>
   </si>
@@ -310,6 +310,15 @@
   </si>
   <si>
     <t>Participant Correct Spelling (Contributor 3)</t>
+  </si>
+  <si>
+    <t>&lt;mods:identifier displayLabel="Digital Folder Number" type="local"&gt;</t>
+  </si>
+  <si>
+    <t>Digital Folder number</t>
+  </si>
+  <si>
+    <t>The Digital Folder number assigned to the interview, for linking to the interview from the Finding Aid</t>
   </si>
 </sst>
 </file>
@@ -396,7 +405,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -405,7 +414,6 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -726,10 +734,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{589D00E9-24EF-4C42-B836-025FE26EDFD9}">
-  <dimension ref="A1:CY1"/>
+  <dimension ref="A1:DB1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="BF1" sqref="BF1"/>
+    <sheetView topLeftCell="CI1" workbookViewId="0">
+      <selection activeCell="DA1" sqref="DA1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -740,7 +748,6 @@
     <col min="14" max="14" width="10" customWidth="1"/>
     <col min="17" max="17" width="15.85546875" customWidth="1"/>
     <col min="20" max="20" width="24.85546875" customWidth="1"/>
-    <col min="23" max="60" width="9.140625" style="8"/>
     <col min="62" max="62" width="9.140625" customWidth="1"/>
     <col min="65" max="65" width="18.5703125" customWidth="1"/>
     <col min="71" max="71" width="11.28515625" customWidth="1"/>
@@ -751,7 +758,7 @@
     <col min="95" max="95" width="18.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:103" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:106" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>18</v>
       </c>
@@ -818,118 +825,118 @@
       <c r="V1" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="W1" s="11" t="s">
+      <c r="W1" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="X1" s="9" t="s">
+      <c r="X1" s="8" t="s">
         <v>80</v>
       </c>
-      <c r="Y1" s="12" t="s">
+      <c r="Y1" s="11" t="s">
         <v>28</v>
       </c>
-      <c r="Z1" s="12" t="s">
+      <c r="Z1" s="11" t="s">
         <v>20</v>
       </c>
-      <c r="AA1" s="9" t="s">
+      <c r="AA1" s="8" t="s">
         <v>81</v>
       </c>
-      <c r="AB1" s="12" t="s">
-        <v>21</v>
-      </c>
-      <c r="AC1" s="12" t="s">
+      <c r="AB1" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="AC1" s="11" t="s">
         <v>48</v>
       </c>
-      <c r="AD1" s="9" t="s">
+      <c r="AD1" s="8" t="s">
         <v>82</v>
       </c>
-      <c r="AE1" s="12" t="s">
-        <v>21</v>
-      </c>
-      <c r="AF1" s="12" t="s">
+      <c r="AE1" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="AF1" s="11" t="s">
         <v>22</v>
       </c>
-      <c r="AG1" s="9" t="s">
+      <c r="AG1" s="8" t="s">
         <v>83</v>
       </c>
-      <c r="AH1" s="12" t="s">
-        <v>21</v>
-      </c>
-      <c r="AI1" s="12" t="s">
+      <c r="AH1" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="AI1" s="11" t="s">
         <v>23</v>
       </c>
-      <c r="AJ1" s="9" t="s">
+      <c r="AJ1" s="8" t="s">
         <v>84</v>
       </c>
-      <c r="AK1" s="12" t="s">
-        <v>21</v>
-      </c>
-      <c r="AL1" s="12" t="s">
+      <c r="AK1" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="AL1" s="11" t="s">
         <v>24</v>
       </c>
-      <c r="AM1" s="9" t="s">
+      <c r="AM1" s="8" t="s">
         <v>85</v>
       </c>
-      <c r="AN1" s="12" t="s">
-        <v>21</v>
-      </c>
-      <c r="AO1" s="12" t="s">
+      <c r="AN1" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="AO1" s="11" t="s">
         <v>25</v>
       </c>
-      <c r="AP1" s="13" t="s">
+      <c r="AP1" s="12" t="s">
         <v>19</v>
       </c>
-      <c r="AQ1" s="10" t="s">
+      <c r="AQ1" s="9" t="s">
         <v>86</v>
       </c>
-      <c r="AR1" s="14" t="s">
+      <c r="AR1" s="13" t="s">
         <v>28</v>
       </c>
-      <c r="AS1" s="14" t="s">
+      <c r="AS1" s="13" t="s">
         <v>20</v>
       </c>
-      <c r="AT1" s="10" t="s">
+      <c r="AT1" s="9" t="s">
         <v>87</v>
       </c>
-      <c r="AU1" s="14" t="s">
-        <v>21</v>
-      </c>
-      <c r="AV1" s="14" t="s">
+      <c r="AU1" s="13" t="s">
+        <v>21</v>
+      </c>
+      <c r="AV1" s="13" t="s">
         <v>48</v>
       </c>
-      <c r="AW1" s="10" t="s">
+      <c r="AW1" s="9" t="s">
         <v>88</v>
       </c>
-      <c r="AX1" s="14" t="s">
-        <v>21</v>
-      </c>
-      <c r="AY1" s="14" t="s">
+      <c r="AX1" s="13" t="s">
+        <v>21</v>
+      </c>
+      <c r="AY1" s="13" t="s">
         <v>22</v>
       </c>
-      <c r="AZ1" s="10" t="s">
+      <c r="AZ1" s="9" t="s">
         <v>89</v>
       </c>
-      <c r="BA1" s="14" t="s">
-        <v>21</v>
-      </c>
-      <c r="BB1" s="14" t="s">
+      <c r="BA1" s="13" t="s">
+        <v>21</v>
+      </c>
+      <c r="BB1" s="13" t="s">
         <v>23</v>
       </c>
-      <c r="BC1" s="10" t="s">
+      <c r="BC1" s="9" t="s">
         <v>90</v>
       </c>
-      <c r="BD1" s="14" t="s">
-        <v>21</v>
-      </c>
-      <c r="BE1" s="14" t="s">
+      <c r="BD1" s="13" t="s">
+        <v>21</v>
+      </c>
+      <c r="BE1" s="13" t="s">
         <v>24</v>
       </c>
-      <c r="BF1" s="10" t="s">
+      <c r="BF1" s="9" t="s">
         <v>91</v>
       </c>
-      <c r="BG1" s="14" t="s">
-        <v>21</v>
-      </c>
-      <c r="BH1" s="14" t="s">
+      <c r="BG1" s="13" t="s">
+        <v>21</v>
+      </c>
+      <c r="BH1" s="13" t="s">
         <v>25</v>
       </c>
       <c r="BI1" t="s">
@@ -1059,6 +1066,15 @@
         <v>43</v>
       </c>
       <c r="CY1" t="s">
+        <v>92</v>
+      </c>
+      <c r="CZ1" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="DA1" t="s">
+        <v>42</v>
+      </c>
+      <c r="DB1" t="s">
         <v>50</v>
       </c>
     </row>
@@ -1070,10 +1086,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CCDD56D4-8BE4-4A5D-B443-4AB7EB265FA6}">
-  <dimension ref="A1:B22"/>
+  <dimension ref="A1:B23"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B22" sqref="B22"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1239,6 +1255,14 @@
         <v>73</v>
       </c>
     </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>93</v>
+      </c>
+      <c r="B23" t="s">
+        <v>94</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
add type of resource constant data
</commit_message>
<xml_diff>
--- a/ExceltoMODSWF/SA-MODS-template.xlsx
+++ b/ExceltoMODSWF/SA-MODS-template.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\goslen\git_repos\box-c-mods-templates\ExceltoMODSWF\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{74121E21-8FC5-4C4D-9440-02A756289549}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{43000CEB-B509-44F7-9D4E-22A2A87AC771}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1845" yWindow="705" windowWidth="24180" windowHeight="14115" activeTab="1" xr2:uid="{30AE1F1C-9D6D-4975-B041-019DDB28DD50}"/>
+    <workbookView xWindow="1560" yWindow="1560" windowWidth="24180" windowHeight="14115" activeTab="1" xr2:uid="{30AE1F1C-9D6D-4975-B041-019DDB28DD50}"/>
   </bookViews>
   <sheets>
     <sheet name="Template" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="95">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="97">
   <si>
     <t>Contributor (Participant) Name</t>
   </si>
@@ -186,9 +186,6 @@
     <t>Ethnic or Racial Identity</t>
   </si>
   <si>
-    <t>&lt;/mods:mods&gt;&lt;/datastream&gt;&lt;/object&gt;</t>
-  </si>
-  <si>
     <t>Notes and Best Practices</t>
   </si>
   <si>
@@ -319,6 +316,15 @@
   </si>
   <si>
     <t>The Digital Folder number assigned to the interview, for linking to the interview from the Finding Aid</t>
+  </si>
+  <si>
+    <t>&lt;mods:typeOfResource&gt;sound recording-nonmusical&lt;/mods:typeOfResource&gt;&lt;/mods:mods&gt;&lt;/datastream&gt;&lt;/object&gt;</t>
+  </si>
+  <si>
+    <t>Type of Resource</t>
+  </si>
+  <si>
+    <t>constant value embedded in template- "sound recording-nonmusical"</t>
   </si>
 </sst>
 </file>
@@ -736,8 +742,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{589D00E9-24EF-4C42-B836-025FE26EDFD9}">
   <dimension ref="A1:DB1"/>
   <sheetViews>
-    <sheetView topLeftCell="CI1" workbookViewId="0">
-      <selection activeCell="DA1" sqref="DA1"/>
+    <sheetView topLeftCell="CF1" workbookViewId="0">
+      <selection activeCell="DB1" sqref="DB1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -766,13 +772,13 @@
         <v>17</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D1" s="5" t="s">
         <v>19</v>
       </c>
       <c r="E1" s="7" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="F1" s="6" t="s">
         <v>28</v>
@@ -781,7 +787,7 @@
         <v>20</v>
       </c>
       <c r="H1" s="7" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="I1" s="6" t="s">
         <v>21</v>
@@ -790,7 +796,7 @@
         <v>48</v>
       </c>
       <c r="K1" s="7" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="L1" s="6" t="s">
         <v>21</v>
@@ -799,7 +805,7 @@
         <v>22</v>
       </c>
       <c r="N1" s="7" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="O1" s="6" t="s">
         <v>21</v>
@@ -808,7 +814,7 @@
         <v>23</v>
       </c>
       <c r="Q1" s="7" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="R1" s="6" t="s">
         <v>21</v>
@@ -817,7 +823,7 @@
         <v>24</v>
       </c>
       <c r="T1" s="7" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="U1" s="6" t="s">
         <v>21</v>
@@ -829,7 +835,7 @@
         <v>19</v>
       </c>
       <c r="X1" s="8" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="Y1" s="11" t="s">
         <v>28</v>
@@ -838,7 +844,7 @@
         <v>20</v>
       </c>
       <c r="AA1" s="8" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="AB1" s="11" t="s">
         <v>21</v>
@@ -847,7 +853,7 @@
         <v>48</v>
       </c>
       <c r="AD1" s="8" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="AE1" s="11" t="s">
         <v>21</v>
@@ -856,7 +862,7 @@
         <v>22</v>
       </c>
       <c r="AG1" s="8" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="AH1" s="11" t="s">
         <v>21</v>
@@ -865,7 +871,7 @@
         <v>23</v>
       </c>
       <c r="AJ1" s="8" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="AK1" s="11" t="s">
         <v>21</v>
@@ -874,7 +880,7 @@
         <v>24</v>
       </c>
       <c r="AM1" s="8" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="AN1" s="11" t="s">
         <v>21</v>
@@ -886,7 +892,7 @@
         <v>19</v>
       </c>
       <c r="AQ1" s="9" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="AR1" s="13" t="s">
         <v>28</v>
@@ -895,7 +901,7 @@
         <v>20</v>
       </c>
       <c r="AT1" s="9" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="AU1" s="13" t="s">
         <v>21</v>
@@ -904,7 +910,7 @@
         <v>48</v>
       </c>
       <c r="AW1" s="9" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="AX1" s="13" t="s">
         <v>21</v>
@@ -913,7 +919,7 @@
         <v>22</v>
       </c>
       <c r="AZ1" s="9" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="BA1" s="13" t="s">
         <v>21</v>
@@ -922,7 +928,7 @@
         <v>23</v>
       </c>
       <c r="BC1" s="9" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="BD1" s="13" t="s">
         <v>21</v>
@@ -931,7 +937,7 @@
         <v>24</v>
       </c>
       <c r="BF1" s="9" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="BG1" s="13" t="s">
         <v>21</v>
@@ -967,7 +973,7 @@
         <v>31</v>
       </c>
       <c r="BR1" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="BS1" s="1" t="s">
         <v>2</v>
@@ -1012,7 +1018,7 @@
         <v>36</v>
       </c>
       <c r="CG1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="CH1" s="3" t="s">
         <v>9</v>
@@ -1021,7 +1027,7 @@
         <v>37</v>
       </c>
       <c r="CJ1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="CK1" s="3" t="s">
         <v>12</v>
@@ -1048,7 +1054,7 @@
         <v>42</v>
       </c>
       <c r="CS1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="CT1" s="1" t="s">
         <v>14</v>
@@ -1057,7 +1063,7 @@
         <v>34</v>
       </c>
       <c r="CV1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="CW1" s="1" t="s">
         <v>15</v>
@@ -1066,16 +1072,16 @@
         <v>43</v>
       </c>
       <c r="CY1" t="s">
+        <v>91</v>
+      </c>
+      <c r="CZ1" s="1" t="s">
         <v>92</v>
-      </c>
-      <c r="CZ1" s="1" t="s">
-        <v>93</v>
       </c>
       <c r="DA1" t="s">
         <v>42</v>
       </c>
       <c r="DB1" t="s">
-        <v>50</v>
+        <v>94</v>
       </c>
     </row>
   </sheetData>
@@ -1086,10 +1092,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CCDD56D4-8BE4-4A5D-B443-4AB7EB265FA6}">
-  <dimension ref="A1:B23"/>
+  <dimension ref="A1:B24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B23" sqref="B23"/>
+      <selection activeCell="B24" sqref="B24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1099,10 +1105,10 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
@@ -1110,7 +1116,7 @@
         <v>17</v>
       </c>
       <c r="B2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
@@ -1118,7 +1124,7 @@
         <v>0</v>
       </c>
       <c r="B3" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
@@ -1151,7 +1157,7 @@
         <v>10</v>
       </c>
       <c r="B9" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
@@ -1159,7 +1165,7 @@
         <v>11</v>
       </c>
       <c r="B10" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
@@ -1167,7 +1173,7 @@
         <v>1</v>
       </c>
       <c r="B11" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
@@ -1175,7 +1181,7 @@
         <v>2</v>
       </c>
       <c r="B12" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
@@ -1183,7 +1189,7 @@
         <v>5</v>
       </c>
       <c r="B13" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
@@ -1191,7 +1197,7 @@
         <v>44</v>
       </c>
       <c r="B14" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
@@ -1199,7 +1205,7 @@
         <v>47</v>
       </c>
       <c r="B15" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
@@ -1212,7 +1218,7 @@
         <v>9</v>
       </c>
       <c r="B17" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
@@ -1220,7 +1226,7 @@
         <v>12</v>
       </c>
       <c r="B18" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
@@ -1228,7 +1234,7 @@
         <v>13</v>
       </c>
       <c r="B19" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
@@ -1236,7 +1242,7 @@
         <v>16</v>
       </c>
       <c r="B20" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
@@ -1244,7 +1250,7 @@
         <v>14</v>
       </c>
       <c r="B21" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
@@ -1252,15 +1258,23 @@
         <v>15</v>
       </c>
       <c r="B22" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
+        <v>92</v>
+      </c>
+      <c r="B23" t="s">
         <v>93</v>
       </c>
-      <c r="B23" t="s">
-        <v>94</v>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>95</v>
+      </c>
+      <c r="B24" t="s">
+        <v>96</v>
       </c>
     </row>
   </sheetData>

</xml_diff>